<commit_message>
added tf_idf to keyword extraction
</commit_message>
<xml_diff>
--- a/named_entities/Named_Entities.xlsx
+++ b/named_entities/Named_Entities.xlsx
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5012019230769231</v>
+        <v>0.5042424242424243</v>
       </c>
     </row>
     <row r="3">
@@ -494,7 +494,7 @@
         <v>130</v>
       </c>
       <c r="E3" t="n">
-        <v>0.15625</v>
+        <v>0.1575757575757576</v>
       </c>
     </row>
     <row r="4">
@@ -512,10 +512,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09134615384615384</v>
+        <v>0.08848484848484849</v>
       </c>
     </row>
     <row r="5">
@@ -533,10 +533,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05408653846153846</v>
+        <v>0.05212121212121212</v>
       </c>
     </row>
     <row r="6">
@@ -554,10 +554,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03846153846153846</v>
+        <v>0.03757575757575757</v>
       </c>
     </row>
     <row r="7">
@@ -566,19 +566,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PERSON</t>
+          <t>ORDINAL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PERSON: People, including fictional</t>
+          <t>ORDINAL: "first", "second", etc.</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03245192307692308</v>
+        <v>0.03151515151515152</v>
       </c>
     </row>
     <row r="8">
@@ -587,19 +587,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ORDINAL</t>
+          <t>DATE</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ORDINAL: "first", "second", etc.</t>
+          <t>DATE: Absolute or relative dates or periods</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>26</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03125</v>
+        <v>0.03151515151515152</v>
       </c>
     </row>
     <row r="9">
@@ -608,19 +608,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>PERSON</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DATE: Absolute or relative dates or periods</t>
+          <t>PERSON: People, including fictional</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03125</v>
+        <v>0.0303030303030303</v>
       </c>
     </row>
     <row r="10">
@@ -641,7 +641,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="n">
-        <v>0.015625</v>
+        <v>0.01575757575757576</v>
       </c>
     </row>
     <row r="11">
@@ -662,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01322115384615385</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="12">
@@ -683,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01081730769230769</v>
+        <v>0.01090909090909091</v>
       </c>
     </row>
     <row r="13">
@@ -704,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>0.009615384615384616</v>
+        <v>0.009696969696969697</v>
       </c>
     </row>
     <row r="14">
@@ -722,10 +722,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" t="n">
-        <v>0.007211538461538462</v>
+        <v>0.008484848484848486</v>
       </c>
     </row>
     <row r="15">
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>0.004807692307692308</v>
+        <v>0.006060606060606061</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>0.001201923076923077</v>
+        <v>0.001212121212121212</v>
       </c>
     </row>
     <row r="17">
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0.001201923076923077</v>
+        <v>0.001212121212121212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>